<commit_message>
Añadir comentario act viterbi
</commit_message>
<xml_diff>
--- a/nlp/actividades/sintax-tag/mia07_t3_tra_resultados_viterbi.xlsx
+++ b/nlp/actividades/sintax-tag/mia07_t3_tra_resultados_viterbi.xlsx
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Fp</t>
+          <t>NCFS000</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -503,20 +503,20 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.005586415856583765</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>SPS00</t>
+          <t>AQ0MS0</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.007871568247054057</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -528,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.05138384827938065</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -540,7 +540,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>AQ0MS0</t>
+          <t>AQ0CS0</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -556,7 +556,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.006755488834678175</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -571,14 +571,14 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>VMIP3S0</t>
+          <t>SPS00</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.001078422914330084</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.007871568247054057</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.05138384827938065</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -602,7 +602,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>NCFS000</t>
+          <t>DA0MS0</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -612,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.6456245689480303</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -633,7 +633,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>NCMP000</t>
+          <t>Fp</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -655,26 +655,26 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.00537109375</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>0.005586415856583765</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>DA0MS0</t>
+          <t>VMIP3S0</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.001078422914330084</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6456245689480303</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -726,7 +726,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>AQ0CS0</t>
+          <t>NCMP000</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -742,13 +742,13 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.006755488834678175</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.00537109375</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>

</xml_diff>